<commit_message>
deliver second round criticalities (rev 3.5 ) to BP
</commit_message>
<xml_diff>
--- a/Waterfall 3.0 to 3.5.xlsx
+++ b/Waterfall 3.0 to 3.5.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://addenergygroup-my.sharepoint.com/personal/douglas_crooke_addenergy_no/Documents/CriticalityVBA/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Douglas.Crooke\OneDrive - add energy group\CriticalityVBA\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4650" yWindow="0" windowWidth="27870" windowHeight="11295" activeTab="3"/>
+    <workbookView xWindow="6510" yWindow="0" windowWidth="27870" windowHeight="11295" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="4" r:id="rId1"/>
@@ -1392,11 +1392,11 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-GB"/>
-              <a:t>Criticality Changes From Systems Feedback (3.0-&gt;3.4), Remove Integrity Only Codes, Make Shutdowns and</a:t>
+              <a:t>WND Criticality Changes From Systems Feedback (3.0-&gt;3.5), Remove Integrity Only Codes, Make Shutdowns and</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-GB" baseline="0"/>
-              <a:t> F&amp;G A</a:t>
+              <a:t> F&amp;G A, Split Lighting</a:t>
             </a:r>
           </a:p>
           <a:p>
@@ -4802,7 +4802,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Chart3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="84" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="84" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="8" orientation="landscape" r:id="rId1"/>
@@ -5028,7 +5028,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="14557963" cy="9219259"/>
+    <xdr:ext cx="14548304" cy="9207500"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -5442,8 +5442,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:J108"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8810,7 +8810,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:Q112"/>
   <sheetViews>
-    <sheetView topLeftCell="A76" workbookViewId="0">
+    <sheetView topLeftCell="A88" workbookViewId="0">
       <selection activeCell="C105" sqref="C105:C107"/>
     </sheetView>
   </sheetViews>

</xml_diff>